<commit_message>
Updated data to reflect new requirement separation
</commit_message>
<xml_diff>
--- a/data/AEPS.xlsx
+++ b/data/AEPS.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -371,6 +371,21 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>Corequisites</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Concurrent</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Recommended</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>Terms Typically Offered</t>
         </is>
       </c>
@@ -393,6 +408,21 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>F</t>
         </is>
       </c>
@@ -415,6 +445,21 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>F, W, SP</t>
         </is>
       </c>
@@ -437,6 +482,21 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>F, W, SP</t>
         </is>
       </c>
@@ -454,10 +514,25 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>AEPS 120.</t>
+          <t>AEPS 120.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>W</t>
         </is>
@@ -476,10 +551,25 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>AEPS 120 and BOT 121.</t>
+          <t>AEPS 120 and BOT 121.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
@@ -498,10 +588,25 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>AEPS 120.</t>
+          <t>AEPS 120.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -525,6 +630,21 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>W</t>
         </is>
       </c>
@@ -542,10 +662,25 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>AEPS 120.</t>
+          <t>AEPS 120.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
         <is>
           <t>W</t>
         </is>
@@ -564,10 +699,25 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>AEPS 132.</t>
+          <t>AEPS 132.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
@@ -591,6 +741,21 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>F</t>
         </is>
       </c>
@@ -613,6 +778,21 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
           <t>F, SP</t>
         </is>
       </c>
@@ -630,10 +810,25 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>AEPS 120.</t>
+          <t>AEPS 120.</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
@@ -657,6 +852,21 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
           <t>F,W,SP,SU</t>
         </is>
       </c>
@@ -679,6 +889,21 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>F, W, SP</t>
         </is>
       </c>
@@ -701,6 +926,21 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
           <t>F, W, SP</t>
         </is>
       </c>
@@ -723,6 +963,21 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
           <t>F, W, SP</t>
         </is>
       </c>
@@ -745,6 +1000,21 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
           <t>F, W</t>
         </is>
       </c>
@@ -762,10 +1032,25 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>AEPS 215.</t>
+          <t>AEPS 215.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
@@ -789,6 +1074,21 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
           <t>F</t>
         </is>
       </c>
@@ -811,6 +1111,21 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
           <t>SP</t>
         </is>
       </c>
@@ -833,6 +1148,21 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
           <t>F</t>
         </is>
       </c>
@@ -850,10 +1180,25 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>AEPS 120 or AEPS 260.</t>
+          <t>AEPS 120 or AEPS 260.</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
@@ -872,10 +1217,25 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>AEPS 133 or AEPS 190 or AEPS 260 or BRAE 237 or BRAE 239.</t>
+          <t>AEPS 133 or AEPS 190 or AEPS 260 or BRAE 237 or BRAE 239.</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
         <is>
           <t>W</t>
         </is>
@@ -899,6 +1259,21 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
           <t>F</t>
         </is>
       </c>
@@ -921,6 +1296,21 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
           <t>TBD</t>
         </is>
       </c>
@@ -938,10 +1328,25 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>AEPS 127, and AEPS 233 or AEPS 234.</t>
+          <t>AEPS 127, and AEPS 233 or AEPS 234.</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -960,12 +1365,27 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>AEPS 120 and STAT 218. Recommended: one of the following: AEPS 132, AEPS 190, AEPS 230, AEPS 245, AEPS 250, or WVIT 233.</t>
+          <t>AEPS 120 and STAT 218.</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>W, SP</t>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>one of the AEPS 132, AEPS 190, AEPS 230, AEPS 245, AEPS 250, or WVIT 233.</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">W, SP </t>
         </is>
       </c>
     </row>
@@ -987,6 +1407,21 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
           <t>F, W, SP</t>
         </is>
       </c>
@@ -1004,10 +1439,25 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>AEPS 120 or BOT 121; and one of the following: CHEM 110, CHEM 111, or CHEM 127.</t>
+          <t>AEPS 120 or BOT 121; and one of the CHEM 110, CHEM 111, or CHEM 127.</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
         <is>
           <t>F, SP</t>
         </is>
@@ -1031,6 +1481,21 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
           <t>F, SP</t>
         </is>
       </c>
@@ -1048,10 +1513,25 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>AEPS 120 or BOT 121.</t>
+          <t>AEPS 120 or BOT 121.</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
         <is>
           <t>F, SP</t>
         </is>
@@ -1070,10 +1550,25 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>BIO 162 or BOT 121.</t>
+          <t>BIO 162 or BOT 121.</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
         <is>
           <t>F, SP</t>
         </is>
@@ -1097,6 +1592,21 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
           <t>W</t>
         </is>
       </c>
@@ -1114,10 +1624,25 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Junior standing; completion of GE Area A with grades of C- or better; completion of one course in GE Area B1 with a grade of C- or better; and one of the following courses: AEPS 120, BIO 111, BIO 114, BIO 161, or BOT 121.</t>
+          <t>Junior standing; completion of GE Area A with grades of C- or better; completion of one course in GE Area B1 with a grade of C- or better; and one of the following AEPS 120, BIO 111, BIO 114, BIO 161, or BOT 121.</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1136,10 +1661,25 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>AEPS/WVIT 231 or WVIT 232 or WVIT 233.</t>
+          <t>AEPS/WVIT 231 or WVIT 232 or WVIT 233.</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
         <is>
           <t>F, SU</t>
         </is>
@@ -1158,10 +1698,25 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>AEPS 126 and AEPS 127.</t>
+          <t>AEPS 126 and AEPS 127.</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -1180,10 +1735,25 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>AEPS 120; CHEM 111 or CHEM 127; and SS 221.</t>
+          <t>AEPS 120; CHEM 111 or CHEM 127; and SS 221.</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1202,10 +1772,25 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>AEPS 333.</t>
+          <t>AEPS 333.</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
         <is>
           <t>W, SP</t>
         </is>
@@ -1229,6 +1814,21 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
           <t>F,W,SP,SU</t>
         </is>
       </c>
@@ -1246,10 +1846,25 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>AEPS 245.</t>
+          <t>AEPS 245.</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
@@ -1268,10 +1883,25 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>AEPS 120.</t>
+          <t>AEPS 120.</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1290,10 +1920,25 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>AEPS 245.</t>
+          <t>AEPS 245.</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
         <is>
           <t>W</t>
         </is>
@@ -1312,10 +1957,25 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>AEPS 120 or BOT 121; and SS 120 or SS 121.</t>
+          <t>AEPS 120 or BOT 121; and SS 120 or SS 121.</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -1334,10 +1994,25 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>AEPS 124; CHEM 111 or CHEM 127; and SS 120 or SS 121.</t>
+          <t>AEPS 124; CHEM 111 or CHEM 127; and SS 120 or SS 121.</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
         <is>
           <t>W</t>
         </is>
@@ -1356,10 +2031,25 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Junior standing and MATH 118 or equivalent, and STAT 218.</t>
+          <t>Junior standing and MATH 118 or equivalent, and STAT 218.</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
         <is>
           <t>W</t>
         </is>
@@ -1378,10 +2068,25 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>AEPS 120 or AEPS 250.</t>
+          <t>AEPS 120 or AEPS 250.</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
@@ -1400,10 +2105,25 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>BIO 114 or BOT 121; and junior standing.</t>
+          <t>BIO 114 or BOT 121; and junior standing.</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
@@ -1427,6 +2147,21 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
           <t>F,W,SP,SU</t>
         </is>
       </c>
@@ -1444,10 +2179,25 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>AEPS 321.</t>
+          <t>AEPS 321.</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
         <is>
           <t>W</t>
         </is>
@@ -1466,10 +2216,25 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>AEPS 120 or BIO 263; BIO 162 or BOT 121; and CHEM 216 or CHEM 312.</t>
+          <t>AEPS 120 or BIO 263; BIO 162 or BOT 121; and CHEM 216 or CHEM 312.</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
@@ -1488,10 +2253,25 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>AEPS/WVIT 231, WVIT 232 or WVIT 233; AEPS 313; AEPS/BOT 323.</t>
+          <t>AEPS/WVIT 231, WVIT 232 or WVIT 233; AEPS 313; AEPS/BOT 323.</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1510,10 +2290,25 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>AEPS 120 or BOT 121; SS 120; and junior standing.</t>
+          <t>AEPS 120 or BOT 121; SS 120; and junior standing.</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
         <is>
           <t>W</t>
         </is>
@@ -1537,6 +2332,21 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
           <t>W</t>
         </is>
       </c>
@@ -1554,10 +2364,25 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>AEPS 190 or AEPS 260.</t>
+          <t>AEPS 190 or AEPS 260.</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -1576,10 +2401,25 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>AEPS 124.</t>
+          <t>AEPS 124.</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
         <is>
           <t>W</t>
         </is>
@@ -1598,10 +2438,25 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>AEPS 123, AEPS 233, and AEPS 234 or NR 208 for FNR majors.</t>
+          <t>AEPS 123, AEPS 233, and AEPS 234 or NR 208 for FNR majors.</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
@@ -1620,10 +2475,25 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>AEPS 120, AEPS 313, AEPS 321, and AEPS/BOT 323.</t>
+          <t>AEPS 120, AEPS 313, AEPS 321, and AEPS/BOT 323.</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
         <is>
           <t>W</t>
         </is>
@@ -1642,10 +2512,25 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>AEPS 313.</t>
+          <t>AEPS 313.</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
@@ -1664,10 +2549,25 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>AEPS 343.</t>
+          <t>AEPS 343.</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -1686,10 +2586,25 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>AEPS 123 and AEPS 126 and junior standing.</t>
+          <t>AEPS 123 and AEPS 126 and junior standing.</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
@@ -1708,12 +2623,27 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>AEPS 233, AEPS 234, AEPS 301. Recommended: AEPS 381.</t>
+          <t>AEPS 233, AEPS 234, AEPS 301.</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>AEPS 381.</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">TBD </t>
         </is>
       </c>
     </row>
@@ -1735,6 +2665,21 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
           <t>TBD</t>
         </is>
       </c>
@@ -1752,10 +2697,25 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>AEPS 313.</t>
+          <t>AEPS 313.</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1774,10 +2734,25 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>AEPS 120; or BOT 121 and SS 120 or SS 121; or graduate standing.</t>
+          <t>AEPS 120; or BOT 121 and SS 120 or SS 121; or graduate standing.</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
         <is>
           <t>W</t>
         </is>
@@ -1796,12 +2771,27 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>AEPS 120. Corequisite: BOT 121.</t>
+          <t>AEPS 120.</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>BOT 121.</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SP </t>
         </is>
       </c>
     </row>
@@ -1818,10 +2808,25 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Junior standing, completion of GE Area A1 with a grade of C- or better, and STAT 218.</t>
+          <t>Junior standing, completion of GE Area A1 with a grade of C- or better, and STAT 218.</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
         <is>
           <t>F, W, SP</t>
         </is>
@@ -1845,6 +2850,21 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
           <t>F,W,SP,SU</t>
         </is>
       </c>
@@ -1867,6 +2887,21 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
           <t>W, SP</t>
         </is>
       </c>
@@ -1889,6 +2924,21 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
           <t>TBD</t>
         </is>
       </c>
@@ -1911,6 +2961,21 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
           <t>F,W,SP,SU</t>
         </is>
       </c>
@@ -1933,6 +2998,21 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
           <t>F,W,SP,SU</t>
         </is>
       </c>
@@ -1955,6 +3035,21 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
           <t>TBD</t>
         </is>
       </c>
@@ -1977,6 +3072,21 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
           <t>TBD</t>
         </is>
       </c>
@@ -1994,12 +3104,27 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Graduate standing. Recommended: a course in basic entomology, plant pathology, and weed science.</t>
+          <t>Graduate standing.</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>a course in basic entomology, plant pathology, and weed science.</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">W </t>
         </is>
       </c>
     </row>
@@ -2021,6 +3146,21 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
           <t>W</t>
         </is>
       </c>
@@ -2043,6 +3183,21 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
           <t>F, W, SP</t>
         </is>
       </c>
@@ -2065,6 +3220,21 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
           <t>F, W, SP</t>
         </is>
       </c>
@@ -2087,6 +3257,21 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
           <t>F, W, SP</t>
         </is>
       </c>
@@ -2108,6 +3293,21 @@
         </is>
       </c>
       <c r="D80" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
         <is>
           <t>F, W, SP</t>
         </is>

</xml_diff>